<commit_message>
patch: added gender to the architecture
</commit_message>
<xml_diff>
--- a/preferences.xlsx
+++ b/preferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronro\PycharmProjects\Auto_Shibuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E156EB1D-8C91-44F7-AB7F-CE516433489A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E856FEC8-BC9D-4606-8916-0AB084D68EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">prefs!$A$1:$C$52</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="61">
   <si>
     <t>עדי אזרזר</t>
   </si>
@@ -194,6 +207,18 @@
   </si>
   <si>
     <t xml:space="preserve">עמית עמר </t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> נקבה</t>
+  </si>
+  <si>
+    <t>נקבה</t>
+  </si>
+  <si>
+    <t>זכר</t>
   </si>
 </sst>
 </file>
@@ -241,10 +266,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,11 +526,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -506,7 +538,7 @@
     <col min="1" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -516,8 +548,12 @@
       <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +563,15 @@
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2">
+        <f>COUNTIF(D2:D54,"זכר")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -538,8 +581,12 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -549,8 +596,12 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -560,8 +611,12 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -571,8 +626,12 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -582,8 +641,12 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -593,19 +656,27 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -615,8 +686,12 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -626,8 +701,12 @@
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -637,19 +716,27 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -659,19 +746,27 @@
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -681,9 +776,13 @@
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -692,8 +791,12 @@
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -703,9 +806,13 @@
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -714,19 +821,27 @@
       <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -736,19 +851,27 @@
       <c r="C21" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -758,30 +881,42 @@
       <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -791,8 +926,12 @@
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
@@ -802,8 +941,12 @@
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -813,19 +956,27 @@
       <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -835,8 +986,12 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -846,8 +1001,12 @@
       <c r="C31" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -857,8 +1016,12 @@
       <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -868,8 +1031,12 @@
       <c r="C33" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -879,20 +1046,28 @@
       <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -901,8 +1076,12 @@
       <c r="C36" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -912,19 +1091,27 @@
       <c r="C37" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -934,8 +1121,12 @@
       <c r="C39" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
@@ -945,8 +1136,12 @@
       <c r="C40" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
@@ -956,8 +1151,12 @@
       <c r="C41" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -967,8 +1166,12 @@
       <c r="C42" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -978,19 +1181,27 @@
       <c r="C43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
@@ -1000,9 +1211,13 @@
       <c r="C45" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1011,20 +1226,28 @@
       <c r="C46" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1033,8 +1256,12 @@
       <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -1044,8 +1271,12 @@
       <c r="C49" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -1055,19 +1286,27 @@
       <c r="C50" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -1077,35 +1316,47 @@
       <c r="C52" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2"/>
+      <c r="D54" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="A51">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>

</xml_diff>